<commit_message>
Añadidas pruebas de accion de seleccion para el bot en el documento de pruebas
</commit_message>
<xml_diff>
--- a/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
+++ b/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Uniovi\TFG\ElFavorDeLasGuerreras\doc\capitulos\Anexos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xamel\Dropbox\Uniovi\TFG\ElFavorDeLasGuerreras\doc\capitulos\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C6D2E6-56B4-4088-8968-1B43880FF7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD91878B-2D58-4860-8F78-23474081B898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4176" yWindow="360" windowWidth="18528" windowHeight="11352" xr2:uid="{91E62D61-3371-49A3-925F-74CADD294985}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{91E62D61-3371-49A3-925F-74CADD294985}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>4 acciones libres</t>
   </si>
@@ -53,6 +53,30 @@
   </si>
   <si>
     <t>Opciones</t>
+  </si>
+  <si>
+    <t>Es de tipo 3</t>
+  </si>
+  <si>
+    <t>Es de tipo 4</t>
+  </si>
+  <si>
+    <t>Todas las cartas son distintas</t>
+  </si>
+  <si>
+    <t>Hay cartas iguales</t>
+  </si>
+  <si>
+    <t>Todas las cartas son iguales</t>
+  </si>
+  <si>
+    <t>Las opciones son distintas</t>
+  </si>
+  <si>
+    <t>Las opciones son iguales</t>
+  </si>
+  <si>
+    <t>Seleccionar accion seleccion</t>
   </si>
   <si>
     <t>Resultado</t>
@@ -122,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +171,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -160,12 +190,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCFEB32-98DF-4F9A-96C0-42E72833AD6E}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,13 +543,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -544,170 +575,362 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>20</v>
+      <c r="F5" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E6" s="4">
         <f>E5+1</f>
         <v>2</v>
       </c>
-      <c r="F6" t="s">
-        <v>20</v>
+      <c r="F6" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E7" s="4">
         <f>E6+1</f>
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>21</v>
+      <c r="F7" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E9" s="4">
         <f>E7+1</f>
         <v>4</v>
       </c>
-      <c r="F9" t="s">
-        <v>20</v>
+      <c r="F9" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E10" s="4">
         <f>E9+1</f>
         <v>5</v>
       </c>
-      <c r="F10" t="s">
-        <v>20</v>
+      <c r="F10" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" ref="E12" si="0">E10+1</f>
         <v>6</v>
       </c>
-      <c r="F12" t="s">
-        <v>20</v>
+      <c r="F12" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" ref="E13:E19" si="1">E12+1</f>
+        <f t="shared" ref="E13" si="1">E12+1</f>
         <v>7</v>
       </c>
-      <c r="F13" t="s">
-        <v>20</v>
+      <c r="F13" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" ref="E15" si="2">E13+1</f>
         <v>8</v>
       </c>
-      <c r="F15" t="s">
-        <v>20</v>
+      <c r="F15" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" ref="E16:E19" si="3">E15+1</f>
+        <f t="shared" ref="E16" si="3">E15+1</f>
         <v>9</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" ref="E18" si="4">E16+1</f>
         <v>10</v>
       </c>
-      <c r="F18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" ref="E19:E20" si="5">E18+1</f>
         <v>11</v>
       </c>
-      <c r="F19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="F20" t="s">
-        <v>21</v>
-      </c>
+      <c r="F20" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="4">
+        <f>E20+1</f>
+        <v>13</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="4">
+        <f>E23+1</f>
+        <v>14</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="4">
+        <f>E24+1</f>
+        <v>15</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="4">
+        <f>E25+1</f>
+        <v>16</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="4">
+        <f>E27+1</f>
+        <v>17</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E61" s="4"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Añadidas pruebas de la red neuronal al documento de pruebas
</commit_message>
<xml_diff>
--- a/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
+++ b/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xamel\Dropbox\Uniovi\TFG\ElFavorDeLasGuerreras\doc\capitulos\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD91878B-2D58-4860-8F78-23474081B898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D9399E-255A-4FF7-AC93-2A0AB8AA3198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{91E62D61-3371-49A3-925F-74CADD294985}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="31">
   <si>
     <t>4 acciones libres</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Las opciones son iguales</t>
+  </si>
+  <si>
+    <t>Red Neuronal Controller</t>
   </si>
   <si>
     <t>Seleccionar accion seleccion</t>
@@ -131,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +144,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,13 +201,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCFEB32-98DF-4F9A-96C0-42E72833AD6E}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,13 +556,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -575,174 +588,174 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4">
         <f>E5+1</f>
         <v>2</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="4">
         <f>E6+1</f>
         <v>3</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" s="4">
         <f>E7+1</f>
         <v>4</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="4">
         <f>E9+1</f>
         <v>5</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" ref="E12" si="0">E10+1</f>
         <v>6</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" ref="E13" si="1">E12+1</f>
         <v>7</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" ref="E15" si="2">E13+1</f>
         <v>8</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" ref="E16" si="3">E15+1</f>
         <v>9</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" ref="E18" si="4">E16+1</f>
         <v>10</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>28</v>
+      <c r="F18" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" ref="E19:E20" si="5">E18+1</f>
         <v>11</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21" s="4"/>
     </row>
@@ -761,7 +774,7 @@
         <v>13</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -773,7 +786,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -785,7 +798,7 @@
         <v>15</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -803,7 +816,7 @@
         <v>16</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -815,122 +828,278 @@
         <v>17</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="4">
+        <f>E28+1</f>
+        <v>18</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="4">
+        <f>E32+1</f>
+        <v>19</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="4">
+        <f>E33+1</f>
+        <v>20</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="4">
+        <f>E34+1</f>
+        <v>21</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="4">
+        <f>E36+1</f>
+        <v>22</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="4">
+        <f t="shared" ref="E39" si="6">E37+1</f>
+        <v>23</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="4">
+        <f t="shared" ref="E40" si="7">E39+1</f>
+        <v>24</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>20</v>
+      </c>
       <c r="E41" s="4"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="4">
+        <f t="shared" ref="E42" si="8">E40+1</f>
+        <v>25</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="4">
+        <f t="shared" ref="E43" si="9">E42+1</f>
+        <v>26</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
       <c r="E44" s="4"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="4">
+        <f t="shared" ref="E45" si="10">E43+1</f>
+        <v>27</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" s="4">
+        <f t="shared" ref="E46:E47" si="11">E45+1</f>
+        <v>28</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" s="4">
+        <f t="shared" si="11"/>
+        <v>29</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
       <c r="E48" s="4"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E50" s="4"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E51" s="4"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E52" s="4"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="4">
+        <f>E47+1</f>
+        <v>30</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="4">
+        <f>E50+1</f>
+        <v>31</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="4">
+        <f>E51+1</f>
+        <v>32</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E54" s="4"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E55" s="4"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E57" s="4"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E58" s="4"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E59" s="4"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E60" s="4"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E61" s="4"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="4">
+        <f>E52+1</f>
+        <v>33</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="4">
+        <f>E54+1</f>
+        <v>34</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D63" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Añadido esqueleto y primera prueba para el controlador del tablero
</commit_message>
<xml_diff>
--- a/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
+++ b/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xamel\Dropbox\Uniovi\TFG\ElFavorDeLasGuerreras\doc\capitulos\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D9399E-255A-4FF7-AC93-2A0AB8AA3198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9744689A-B48A-4564-B1F0-5665BB64A622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{91E62D61-3371-49A3-925F-74CADD294985}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="34">
   <si>
     <t>4 acciones libres</t>
   </si>
@@ -46,6 +46,9 @@
     <t>Seleccionar accion</t>
   </si>
   <si>
+    <t>Tablero</t>
+  </si>
+  <si>
     <t>Clase</t>
   </si>
   <si>
@@ -128,6 +131,12 @@
   </si>
   <si>
     <t>Exception</t>
+  </si>
+  <si>
+    <t>Crear tablero</t>
+  </si>
+  <si>
+    <t>Todo vacío excepto las manos de los jugadores</t>
   </si>
 </sst>
 </file>
@@ -201,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -209,7 +218,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,17 +540,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCFEB32-98DF-4F9A-96C0-42E72833AD6E}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" customWidth="1"/>
     <col min="4" max="4" width="24.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
@@ -547,22 +558,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -588,252 +599,252 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="4">
         <f>E5+1</f>
         <v>2</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="4">
         <f>E6+1</f>
         <v>3</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E9" s="4">
         <f>E7+1</f>
         <v>4</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E10" s="4">
         <f>E9+1</f>
         <v>5</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" ref="E12" si="0">E10+1</f>
         <v>6</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" ref="E13" si="1">E12+1</f>
         <v>7</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" ref="E15" si="2">E13+1</f>
         <v>8</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" ref="E16" si="3">E15+1</f>
         <v>9</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" ref="E18" si="4">E16+1</f>
         <v>10</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" ref="E19:E20" si="5">E18+1</f>
         <v>11</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E23" s="4">
         <f>E20+1</f>
         <v>13</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E24" s="4">
         <f>E23+1</f>
         <v>14</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E25" s="4">
         <f>E24+1</f>
         <v>15</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E27" s="4">
         <f>E25+1</f>
         <v>16</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E28" s="4">
         <f>E27+1</f>
         <v>17</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -854,252 +865,280 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E32" s="4">
         <f>E28+1</f>
         <v>18</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E33" s="4">
         <f>E32+1</f>
         <v>19</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E34" s="4">
         <f>E33+1</f>
         <v>20</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E35" s="4"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E36" s="4">
         <f>E34+1</f>
         <v>21</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E37" s="4">
         <f>E36+1</f>
         <v>22</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E39" s="4">
         <f t="shared" ref="E39" si="6">E37+1</f>
         <v>23</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E40" s="4">
         <f t="shared" ref="E40" si="7">E39+1</f>
         <v>24</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E41" s="4"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E42" s="4">
         <f t="shared" ref="E42" si="8">E40+1</f>
         <v>25</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E43" s="4">
         <f t="shared" ref="E43" si="9">E42+1</f>
         <v>26</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E44" s="4"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E45" s="4">
         <f t="shared" ref="E45" si="10">E43+1</f>
         <v>27</v>
       </c>
-      <c r="F45" s="6" t="s">
-        <v>29</v>
+      <c r="F45" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E46" s="4">
         <f t="shared" ref="E46:E47" si="11">E45+1</f>
         <v>28</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E47" s="4">
         <f t="shared" si="11"/>
         <v>29</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E48" s="4"/>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E50" s="4">
         <f>E47+1</f>
         <v>30</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E51" s="4">
         <f>E50+1</f>
         <v>31</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E52" s="4">
         <f>E51+1</f>
         <v>32</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E53" s="4"/>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E54" s="4">
         <f>E52+1</f>
         <v>33</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E55" s="4">
         <f>E54+1</f>
         <v>34</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D63" s="7"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>32</v>
+      </c>
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C58" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="4">
+        <f>E55+1</f>
+        <v>35</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D64" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Añadidas pruebas del tablero al documento de pruebas
</commit_message>
<xml_diff>
--- a/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
+++ b/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xamel\Dropbox\Uniovi\TFG\ElFavorDeLasGuerreras\doc\capitulos\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9744689A-B48A-4564-B1F0-5665BB64A622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BB3D2B-64BC-44F6-AC48-D4F53CBF657A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{91E62D61-3371-49A3-925F-74CADD294985}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="74">
   <si>
     <t>4 acciones libres</t>
   </si>
@@ -49,6 +49,15 @@
     <t>Tablero</t>
   </si>
   <si>
+    <t>Robar carta</t>
+  </si>
+  <si>
+    <t>Vista del tablero</t>
+  </si>
+  <si>
+    <t>Realizar accion</t>
+  </si>
+  <si>
     <t>Clase</t>
   </si>
   <si>
@@ -85,6 +94,21 @@
     <t>Seleccionar accion seleccion</t>
   </si>
   <si>
+    <t>Hay accion pendiente</t>
+  </si>
+  <si>
+    <t>Finalizar turno</t>
+  </si>
+  <si>
+    <t>No se ve la mano del adversario</t>
+  </si>
+  <si>
+    <t>Tiene la mano medio llena</t>
+  </si>
+  <si>
+    <t>Tiene la mano llena</t>
+  </si>
+  <si>
     <t>Resultado</t>
   </si>
   <si>
@@ -137,13 +161,109 @@
   </si>
   <si>
     <t>Todo vacío excepto las manos de los jugadores</t>
+  </si>
+  <si>
+    <t>No se han completado todas las acciones</t>
+  </si>
+  <si>
+    <t>Gana el jugador 1</t>
+  </si>
+  <si>
+    <t>Gana el jugador 2</t>
+  </si>
+  <si>
+    <t>Empate</t>
+  </si>
+  <si>
+    <t>Tiene la mano con un solo hueco</t>
+  </si>
+  <si>
+    <t>Iniciar ronda</t>
+  </si>
+  <si>
+    <t>Primera ronda</t>
+  </si>
+  <si>
+    <t>No primera ronda</t>
+  </si>
+  <si>
+    <t>Todo vacío excepto las manos de los jugadores y el favor</t>
+  </si>
+  <si>
+    <t>Todo vacío</t>
+  </si>
+  <si>
+    <t>Inicio primera ronda</t>
+  </si>
+  <si>
+    <t>Se ve la mano del jugador</t>
+  </si>
+  <si>
+    <t>Todo lo demas esta vacio</t>
+  </si>
+  <si>
+    <t>Se ven las acciones del adbersario pero no las cartas</t>
+  </si>
+  <si>
+    <t>Se ven las armas en las guerreras</t>
+  </si>
+  <si>
+    <t>Mitad de la segunda ronda</t>
+  </si>
+  <si>
+    <t>Se ve el favor de las guerreras</t>
+  </si>
+  <si>
+    <t>Se ven las cartas de las acciones del jugador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El tipo de accion esta disponible </t>
+  </si>
+  <si>
+    <t>El tipo de accion no esta disponible</t>
+  </si>
+  <si>
+    <t>La accion esta bien formada</t>
+  </si>
+  <si>
+    <t>La accion esta mal formada</t>
+  </si>
+  <si>
+    <t>Hay una accion pendiente y devuelve true</t>
+  </si>
+  <si>
+    <t>No hay una accion pendiente y devuelve false</t>
+  </si>
+  <si>
+    <t>Tipo secreto</t>
+  </si>
+  <si>
+    <t>Tipo renuncia</t>
+  </si>
+  <si>
+    <t>Tipo regalo</t>
+  </si>
+  <si>
+    <t>Tipo competicion</t>
+  </si>
+  <si>
+    <t>Tipo decision regalo</t>
+  </si>
+  <si>
+    <t>Tipo decision competicion</t>
+  </si>
+  <si>
+    <t>El tipo de accion es el esperado</t>
+  </si>
+  <si>
+    <t>El tipo de accion no es el esperado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,9 +278,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -210,17 +342,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,40 +698,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCFEB32-98DF-4F9A-96C0-42E72833AD6E}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.109375" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="47.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -581,10 +739,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -592,265 +750,265 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="D5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="12">
         <v>1</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>30</v>
+      <c r="F5" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="D6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="12">
         <f>E5+1</f>
         <v>2</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>30</v>
+      <c r="F6" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="D7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="12">
         <f>E6+1</f>
         <v>3</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>31</v>
+      <c r="F7" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="4"/>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="D9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="12">
         <f>E7+1</f>
         <v>4</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>30</v>
+      <c r="F9" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="D10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="12">
         <f>E9+1</f>
         <v>5</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>30</v>
+      <c r="F10" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="4"/>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="D12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="12">
         <f t="shared" ref="E12" si="0">E10+1</f>
         <v>6</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>30</v>
+      <c r="F12" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="D13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="12">
         <f t="shared" ref="E13" si="1">E12+1</f>
         <v>7</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>30</v>
+      <c r="F13" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="4"/>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="4">
+      <c r="D15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="12">
         <f t="shared" ref="E15" si="2">E13+1</f>
         <v>8</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>30</v>
+      <c r="F15" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="4">
+      <c r="D16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="12">
         <f t="shared" ref="E16" si="3">E15+1</f>
         <v>9</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="4">
+      <c r="D18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="12">
         <f t="shared" ref="E18" si="4">E16+1</f>
         <v>10</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>30</v>
+      <c r="F18" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="4">
+      <c r="D19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="12">
         <f t="shared" ref="E19:E20" si="5">E18+1</f>
         <v>11</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>30</v>
+      <c r="F19" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="4">
+      <c r="C20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="12">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>31</v>
+      <c r="F20" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="4"/>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="12"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="4">
+      <c r="D23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="12">
         <f>E20+1</f>
         <v>13</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>30</v>
+      <c r="F23" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="4">
+      <c r="D24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="12">
         <f>E23+1</f>
         <v>14</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>30</v>
+      <c r="F24" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="4">
+      <c r="D25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="12">
         <f>E24+1</f>
         <v>15</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>30</v>
+      <c r="F25" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="4"/>
+      <c r="C26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="4">
+      <c r="D27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="12">
         <f>E25+1</f>
         <v>16</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>30</v>
+      <c r="F27" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="4">
+      <c r="D28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="12">
         <f>E27+1</f>
         <v>17</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>30</v>
+      <c r="F28" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
@@ -858,255 +1016,255 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
+      <c r="C31" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D32" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="4">
+      <c r="D32" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="12">
         <f>E28+1</f>
         <v>18</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>30</v>
+      <c r="F32" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="4">
+      <c r="D33" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="12">
         <f>E32+1</f>
         <v>19</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>30</v>
+      <c r="F33" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="4">
+      <c r="D34" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="12">
         <f>E33+1</f>
         <v>20</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>31</v>
+      <c r="F34" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C35" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="4"/>
+      <c r="C35" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" s="12"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D36" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" s="4">
+      <c r="D36" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="12">
         <f>E34+1</f>
         <v>21</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>30</v>
+      <c r="F36" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D37" t="s">
-        <v>25</v>
-      </c>
-      <c r="E37" s="4">
+      <c r="D37" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="12">
         <f>E36+1</f>
         <v>22</v>
       </c>
-      <c r="F37" s="5" t="s">
-        <v>30</v>
+      <c r="F37" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" s="4"/>
+      <c r="C38" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="12"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D39" t="s">
-        <v>24</v>
-      </c>
-      <c r="E39" s="4">
+      <c r="D39" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" s="12">
         <f t="shared" ref="E39" si="6">E37+1</f>
         <v>23</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>30</v>
+      <c r="F39" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E40" s="4">
+      <c r="D40" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="12">
         <f t="shared" ref="E40" si="7">E39+1</f>
         <v>24</v>
       </c>
-      <c r="F40" s="5" t="s">
-        <v>30</v>
+      <c r="F40" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
-        <v>21</v>
-      </c>
-      <c r="E41" s="4"/>
+      <c r="C41" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="12"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D42" t="s">
-        <v>24</v>
-      </c>
-      <c r="E42" s="4">
+      <c r="D42" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" s="12">
         <f t="shared" ref="E42" si="8">E40+1</f>
         <v>25</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>30</v>
+      <c r="F42" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D43" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" s="4">
+      <c r="D43" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E43" s="12">
         <f t="shared" ref="E43" si="9">E42+1</f>
         <v>26</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F43" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C44" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C44" t="s">
-        <v>22</v>
-      </c>
-      <c r="E44" s="4"/>
+      <c r="E44" s="12"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D45" t="s">
-        <v>24</v>
-      </c>
-      <c r="E45" s="4">
+      <c r="D45" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="12">
         <f t="shared" ref="E45" si="10">E43+1</f>
         <v>27</v>
       </c>
-      <c r="F45" s="7" t="s">
-        <v>30</v>
+      <c r="F45" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E46" s="4">
+      <c r="D46" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" s="12">
         <f t="shared" ref="E46:E47" si="11">E45+1</f>
         <v>28</v>
       </c>
-      <c r="F46" s="5" t="s">
-        <v>30</v>
+      <c r="F46" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
-        <v>29</v>
-      </c>
-      <c r="E47" s="4">
+      <c r="C47" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" s="12">
         <f t="shared" si="11"/>
         <v>29</v>
       </c>
-      <c r="F47" s="5" t="s">
-        <v>31</v>
+      <c r="F47" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>15</v>
-      </c>
-      <c r="E48" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="E48" s="12"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="4"/>
+      <c r="C49" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="12"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D50" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="4">
+      <c r="D50" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="12">
         <f>E47+1</f>
         <v>30</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>30</v>
+      <c r="F50" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D51" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" s="4">
+      <c r="D51" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="12">
         <f>E50+1</f>
         <v>31</v>
       </c>
-      <c r="F51" s="5" t="s">
-        <v>30</v>
+      <c r="F51" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D52" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="4">
+      <c r="D52" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" s="12">
         <f>E51+1</f>
         <v>32</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>30</v>
+      <c r="F52" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="4"/>
+      <c r="C53" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="12"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D54" t="s">
-        <v>12</v>
-      </c>
-      <c r="E54" s="4">
+      <c r="D54" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="12">
         <f>E52+1</f>
         <v>33</v>
       </c>
-      <c r="F54" s="5" t="s">
-        <v>30</v>
+      <c r="F54" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D55" t="s">
-        <v>13</v>
-      </c>
-      <c r="E55" s="4">
+      <c r="D55" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="12">
         <f>E54+1</f>
         <v>34</v>
       </c>
-      <c r="F55" s="5" t="s">
-        <v>30</v>
+      <c r="F55" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1114,31 +1272,371 @@
         <v>3</v>
       </c>
       <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="14"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>32</v>
-      </c>
-      <c r="E57" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="E57" s="12"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C58" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E58" s="4">
-        <f>E55+1</f>
-        <v>35</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="C58" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E58" s="7"/>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>47</v>
+      </c>
+      <c r="E59" s="7"/>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C60" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E60" s="7"/>
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D61" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E61" s="7"/>
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C62" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E62" s="7"/>
+      <c r="F62" s="8"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D63" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E63" s="7"/>
+      <c r="F63" s="8"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D64" s="9"/>
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" s="7"/>
+      <c r="F64" s="8"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C65" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E65" s="7"/>
+      <c r="F65" s="8"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D66" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E66" s="7"/>
+      <c r="F66" s="8"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D67" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="7"/>
+      <c r="F67" s="8"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D68" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E68" s="7"/>
+      <c r="F68" s="8"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C69" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E69" s="7"/>
+      <c r="F69" s="8"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D70" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E70" s="7"/>
+      <c r="F70" s="8"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D71" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="7"/>
+      <c r="F71" s="8"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D72" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E72" s="7"/>
+      <c r="F72" s="8"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D73" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E73" s="7"/>
+      <c r="F73" s="8"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D74" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E74" s="7"/>
+      <c r="F74" s="8"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D75" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E75" s="7"/>
+      <c r="F75" s="8"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76" s="7"/>
+      <c r="F76" s="8"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C77" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E77" s="7"/>
+      <c r="F77" s="8"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C78" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E78" s="7"/>
+      <c r="F78" s="8"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C79" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E79" s="7"/>
+      <c r="F79" s="8"/>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" s="7"/>
+      <c r="F80" s="8"/>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C81" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E81" s="7"/>
+      <c r="F81" s="8"/>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D82" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D83" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D84" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D85" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C86" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D87" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D88" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D89" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D90" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C91" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D92" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D93" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D94" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="95" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D95" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="96" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C96" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D97" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D98" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D99" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D100" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C101" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D101" s="6"/>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D102" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D103" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D104" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D105" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C106" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D107" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D108" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D109" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D110" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C112" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C113" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>20</v>
+      </c>
+      <c r="E114" s="12"/>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C115" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C116" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C117" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C118" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Añadidos test 45, 46 y 47 junto a comprobaciones en la aplicación que faltaban
</commit_message>
<xml_diff>
--- a/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
+++ b/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xamel\Dropbox\Uniovi\TFG\ElFavorDeLasGuerreras\doc\capitulos\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414FD77D-F985-461E-99BC-57453843120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D042EE1-C287-4C06-AC13-9BFCEB3F82A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{91E62D61-3371-49A3-925F-74CADD294985}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="80">
   <si>
     <t>4 acciones libres</t>
   </si>
@@ -103,9 +103,6 @@
     <t>ObtenerPrediccionCampo</t>
   </si>
   <si>
-    <t>Hay accion pendiente</t>
-  </si>
-  <si>
     <t>Finalizar turno</t>
   </si>
   <si>
@@ -229,15 +226,6 @@
     <t>La accion esta bien formada</t>
   </si>
   <si>
-    <t>La accion esta mal formada</t>
-  </si>
-  <si>
-    <t>Hay una accion pendiente y devuelve true</t>
-  </si>
-  <si>
-    <t>No hay una accion pendiente y devuelve false</t>
-  </si>
-  <si>
     <t>Tipo secreto</t>
   </si>
   <si>
@@ -284,6 +272,9 @@
   </si>
   <si>
     <t>El mazo esta vacio</t>
+  </si>
+  <si>
+    <t>La accion tiene un numero incorrecto de cartas</t>
   </si>
 </sst>
 </file>
@@ -721,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCFEB32-98DF-4F9A-96C0-42E72833AD6E}">
-  <dimension ref="A1:S130"/>
+  <dimension ref="A1:S127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="I82" sqref="I82"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="I96" sqref="I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,16 +740,16 @@
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -786,54 +777,54 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="8">
         <v>1</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="S5" s="18"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="8">
         <f>E5+1</f>
         <v>2</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="S6" s="18"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="8">
         <f>E6+1</f>
         <v>3</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="S7" s="18"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="10"/>
@@ -841,39 +832,39 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="8">
         <f>E7+1</f>
         <v>4</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="S9" s="18"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="8">
         <f>E9+1</f>
         <v>5</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="S10" s="18"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="10"/>
@@ -881,39 +872,39 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="8">
         <f t="shared" ref="E12" si="0">E10+1</f>
         <v>6</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="S12" s="18"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D13" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="8">
         <f t="shared" ref="E13" si="1">E12+1</f>
         <v>7</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="S13" s="18"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="10"/>
@@ -921,84 +912,84 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="8">
         <f t="shared" ref="E15" si="2">E13+1</f>
         <v>8</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="8">
         <f t="shared" ref="E16" si="3">E15+1</f>
         <v>9</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="8">
         <f t="shared" ref="E18" si="4">E16+1</f>
         <v>10</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="8">
         <f t="shared" ref="E19:E20" si="5">E18+1</f>
         <v>11</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="8">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1024,10 +1015,10 @@
         <v>13</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1039,10 +1030,10 @@
         <v>14</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1054,10 +1045,10 @@
         <v>15</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1076,10 +1067,10 @@
         <v>16</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1091,10 +1082,10 @@
         <v>17</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -1121,210 +1112,210 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D32" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E32" s="8">
         <f>E28+1</f>
         <v>18</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D33" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E33" s="8">
         <f>E32+1</f>
         <v>19</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D34" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E34" s="8">
         <f>E33+1</f>
         <v>20</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C35" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="10"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D36" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E36" s="8">
         <f>E34+1</f>
         <v>21</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E37" s="8">
         <f>E36+1</f>
         <v>22</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="10"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D39" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E39" s="8">
         <f t="shared" ref="E39" si="6">E37+1</f>
         <v>23</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D40" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E40" s="8">
         <f t="shared" ref="E40" si="7">E39+1</f>
         <v>24</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="10"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D42" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E42" s="8">
         <f t="shared" ref="E42" si="8">E40+1</f>
         <v>25</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D43" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E43" s="8">
         <f t="shared" ref="E43" si="9">E42+1</f>
         <v>26</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="10"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D45" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E45" s="8">
         <f t="shared" ref="E45" si="10">E43+1</f>
         <v>27</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D46" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E46" s="8">
         <f t="shared" ref="E46:E47" si="11">E45+1</f>
         <v>28</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C47" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E47" s="8">
         <f t="shared" si="11"/>
         <v>29</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
@@ -1350,10 +1341,10 @@
         <v>30</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -1365,10 +1356,10 @@
         <v>31</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -1380,10 +1371,10 @@
         <v>32</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -1402,10 +1393,10 @@
         <v>33</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -1417,10 +1408,10 @@
         <v>34</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -1434,74 +1425,74 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F57" s="10"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C58" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E58" s="8">
         <f>E55+1</f>
         <v>35</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C60" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="5"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D61" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E61" s="8">
         <f>E58+1</f>
         <v>36</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C62" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="5"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D63" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E63" s="8">
         <f>E61+1</f>
         <v>37</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -1513,238 +1504,238 @@
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C65" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D66" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E66" s="8">
         <f>E61</f>
         <v>36</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D67" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E67" s="8">
         <f>E61</f>
         <v>36</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D68" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E68" s="8">
         <f>E61</f>
         <v>36</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C69" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D70" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E70" s="8">
         <f>E63+1</f>
         <v>38</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D71" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E71" s="8">
         <f>E70</f>
         <v>38</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D72" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E72" s="8">
         <f>E70</f>
         <v>38</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D73" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E73" s="8">
         <f>E70</f>
         <v>38</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D74" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E74" s="8">
         <f>E70</f>
         <v>38</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C75" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="10"/>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D76" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E76" s="8">
         <f>E70+1</f>
         <v>39</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D77" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E77" s="8">
         <f>E76</f>
         <v>39</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D78" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E78" s="8">
         <f>E77</f>
         <v>39</v>
       </c>
       <c r="F78" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D79" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E79" s="8">
         <f>E78</f>
         <v>39</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D80" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E80" s="8">
         <f>E79</f>
         <v>39</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D81" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E81" s="8">
         <f>E80</f>
         <v>39</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C82" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.3">
@@ -1756,10 +1747,10 @@
         <v>40</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.3">
@@ -1771,10 +1762,10 @@
         <v>41</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.3">
@@ -1786,47 +1777,47 @@
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C86" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E86" s="8">
         <f>E84+1</f>
         <v>42</v>
       </c>
       <c r="F86" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C87" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E87" s="8">
         <f>E86+1</f>
         <v>43</v>
       </c>
       <c r="F87" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C88" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E88" s="8">
         <f>E87+1</f>
         <v>44</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.3">
@@ -1838,21 +1829,24 @@
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C90" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E90" s="8"/>
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D91" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E91" s="7">
         <f>E88+1</f>
         <v>45</v>
       </c>
       <c r="F91" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.3">
@@ -1860,53 +1854,62 @@
         <v>62</v>
       </c>
       <c r="E92" s="7">
-        <f>E91+1</f>
-        <v>46</v>
+        <f>E91</f>
+        <v>45</v>
       </c>
       <c r="F92" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D93" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E93" s="7">
         <f t="shared" ref="E93:E94" si="12">E92+1</f>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F93" s="10" t="s">
         <v>39</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D94" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="E94" s="7">
         <f t="shared" si="12"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C95" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F95" s="10"/>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D96" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E96" s="7">
         <f>E94+1</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="97" spans="3:6" x14ac:dyDescent="0.3">
@@ -1914,20 +1917,20 @@
         <v>62</v>
       </c>
       <c r="E97" s="7">
-        <f>E96+1</f>
-        <v>50</v>
+        <f>E96</f>
+        <v>48</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="98" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D98" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E98" s="7">
         <f t="shared" ref="E98:E99" si="13">E97+1</f>
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F98" s="10" t="s">
         <v>39</v>
@@ -1935,33 +1938,33 @@
     </row>
     <row r="99" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D99" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="E99" s="7">
         <f t="shared" si="13"/>
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F99" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="100" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C100" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="10"/>
     </row>
     <row r="101" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D101" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E101" s="7">
         <f>E99+1</f>
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F101" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="102" spans="3:6" x14ac:dyDescent="0.3">
@@ -1969,20 +1972,20 @@
         <v>62</v>
       </c>
       <c r="E102" s="7">
-        <f>E101+1</f>
-        <v>54</v>
+        <f>E101</f>
+        <v>51</v>
       </c>
       <c r="F102" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="103" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D103" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E103" s="7">
         <f t="shared" ref="E103:E104" si="14">E102+1</f>
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F103" s="10" t="s">
         <v>39</v>
@@ -1990,32 +1993,32 @@
     </row>
     <row r="104" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D104" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="E104" s="7">
         <f t="shared" si="14"/>
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F104" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="105" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C105" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F105" s="10"/>
     </row>
     <row r="106" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D106" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E106" s="7">
         <f>E104+1</f>
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F106" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="107" spans="3:6" x14ac:dyDescent="0.3">
@@ -2023,20 +2026,20 @@
         <v>62</v>
       </c>
       <c r="E107" s="7">
-        <f>E106+1</f>
-        <v>58</v>
+        <f>E106</f>
+        <v>54</v>
       </c>
       <c r="F107" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="108" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D108" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E108" s="7">
         <f t="shared" ref="E108:E109" si="15">E107+1</f>
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F108" s="10" t="s">
         <v>39</v>
@@ -2044,54 +2047,54 @@
     </row>
     <row r="109" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D109" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="E109" s="7">
         <f t="shared" si="15"/>
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F109" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="110" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C110" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D110" s="4"/>
       <c r="F110" s="10"/>
     </row>
     <row r="111" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D111" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E111" s="7">
         <f>E109+1</f>
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F111" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="112" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D112" s="3" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E112" s="7">
-        <f>E111+1</f>
-        <v>62</v>
+        <f>E111</f>
+        <v>57</v>
       </c>
       <c r="F112" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D113" s="3" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E113" s="7">
         <f t="shared" ref="E113:E114" si="16">E112+1</f>
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F113" s="10" t="s">
         <v>39</v>
@@ -2099,54 +2102,54 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D114" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="E114" s="7">
         <f t="shared" si="16"/>
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F114" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C115" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E115" s="8"/>
       <c r="F115" s="10"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D116" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E116" s="7">
         <f>E114+1</f>
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F116" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D117" s="3" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E117" s="7">
-        <f>E116+1</f>
-        <v>66</v>
+        <f>E116</f>
+        <v>60</v>
       </c>
       <c r="F117" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D118" s="3" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="E118" s="7">
         <f t="shared" ref="E118:E119" si="17">E117+1</f>
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F118" s="10" t="s">
         <v>39</v>
@@ -2154,94 +2157,72 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D119" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="E119" s="7">
         <f t="shared" si="17"/>
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F119" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>22</v>
       </c>
+      <c r="E120" s="8"/>
       <c r="F120" s="10"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C121" s="3" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="F121" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C122" s="3" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="F122" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B123" t="s">
-        <v>23</v>
-      </c>
-      <c r="E123" s="8"/>
-      <c r="F123" s="10"/>
+      <c r="C123" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F123" s="10" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C124" s="3" t="s">
-        <v>43</v>
+      <c r="C124" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="F124" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C125" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F125" s="10" t="s">
-        <v>39</v>
-      </c>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
+      <c r="E125" s="16"/>
+      <c r="F125" s="17"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C126" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F126" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="B126" t="s">
+        <v>20</v>
+      </c>
+      <c r="F126" s="10"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C127" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F127" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C128" s="15"/>
-      <c r="D128" s="15"/>
-      <c r="E128" s="16"/>
-      <c r="F128" s="17"/>
-    </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B129" t="s">
-        <v>20</v>
-      </c>
-      <c r="F129" s="10"/>
-    </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B130" t="s">
+      <c r="B127" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Añadidas pruebas hasta la 56
</commit_message>
<xml_diff>
--- a/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
+++ b/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xamel\Dropbox\Uniovi\TFG\ElFavorDeLasGuerreras\doc\capitulos\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D042EE1-C287-4C06-AC13-9BFCEB3F82A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF647A6-7147-4D42-B791-8667B93317D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{91E62D61-3371-49A3-925F-74CADD294985}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="77">
   <si>
     <t>4 acciones libres</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Realizar accion</t>
   </si>
   <si>
-    <t>Prediccion</t>
-  </si>
-  <si>
     <t>Clase</t>
   </si>
   <si>
@@ -95,12 +92,6 @@
   </si>
   <si>
     <t>Seleccionar accion seleccion</t>
-  </si>
-  <si>
-    <t>Predecir</t>
-  </si>
-  <si>
-    <t>ObtenerPrediccionCampo</t>
   </si>
   <si>
     <t>Finalizar turno</t>
@@ -712,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCFEB32-98DF-4F9A-96C0-42E72833AD6E}">
-  <dimension ref="A1:S127"/>
+  <dimension ref="A1:S124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="I96" sqref="I96"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="G104" sqref="G101:G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,25 +722,25 @@
   <sheetData>
     <row r="1" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -777,54 +768,54 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E5" s="8">
         <v>1</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S5" s="18"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E6" s="8">
         <f>E5+1</f>
         <v>2</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S6" s="18"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D7" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E7" s="8">
         <f>E6+1</f>
         <v>3</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S7" s="18"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="10"/>
@@ -832,39 +823,39 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E9" s="8">
         <f>E7+1</f>
         <v>4</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S9" s="18"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="8">
         <f>E9+1</f>
         <v>5</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S10" s="18"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="10"/>
@@ -872,39 +863,39 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D12" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" s="8">
         <f t="shared" ref="E12" si="0">E10+1</f>
         <v>6</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S12" s="18"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D13" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E13" s="8">
         <f t="shared" ref="E13" si="1">E12+1</f>
         <v>7</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="S13" s="18"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="10"/>
@@ -912,185 +903,185 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D15" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E15" s="8">
         <f t="shared" ref="E15" si="2">E13+1</f>
         <v>8</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D16" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E16" s="8">
         <f t="shared" ref="E16" si="3">E15+1</f>
         <v>9</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D18" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E18" s="8">
         <f t="shared" ref="E18" si="4">E16+1</f>
         <v>10</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D19" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E19" s="8">
         <f t="shared" ref="E19:E20" si="5">E18+1</f>
         <v>11</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E20" s="8">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D23" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" s="8">
         <f>E20+1</f>
         <v>13</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D24" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24" s="8">
         <f>E23+1</f>
         <v>14</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" s="8">
         <f>E24+1</f>
         <v>15</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="10"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E27" s="8">
         <f>E25+1</f>
         <v>16</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D28" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E28" s="8">
         <f>E27+1</f>
         <v>17</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -1112,306 +1103,306 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D32" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E32" s="8">
         <f>E28+1</f>
         <v>18</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D33" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E33" s="8">
         <f>E32+1</f>
         <v>19</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D34" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E34" s="8">
         <f>E33+1</f>
         <v>20</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C35" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="10"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D36" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E36" s="8">
         <f>E34+1</f>
         <v>21</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D37" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E37" s="8">
         <f>E36+1</f>
         <v>22</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="10"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D39" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E39" s="8">
         <f t="shared" ref="E39" si="6">E37+1</f>
         <v>23</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D40" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E40" s="8">
         <f t="shared" ref="E40" si="7">E39+1</f>
         <v>24</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="10"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D42" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E42" s="8">
         <f t="shared" ref="E42" si="8">E40+1</f>
         <v>25</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D43" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E43" s="8">
         <f t="shared" ref="E43" si="9">E42+1</f>
         <v>26</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="10"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D45" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E45" s="8">
         <f t="shared" ref="E45" si="10">E43+1</f>
         <v>27</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D46" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E46" s="8">
         <f t="shared" ref="E46:E47" si="11">E45+1</f>
         <v>28</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C47" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E47" s="8">
         <f t="shared" si="11"/>
         <v>29</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="10"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C49" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E49" s="8"/>
       <c r="F49" s="10"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D50" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E50" s="8">
         <f>E47+1</f>
         <v>30</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D51" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E51" s="8">
         <f>E50+1</f>
         <v>31</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D52" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E52" s="8">
         <f>E51+1</f>
         <v>32</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C53" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="10"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D54" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E54" s="8">
         <f>E52+1</f>
         <v>33</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D55" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E55" s="8">
         <f>E54+1</f>
         <v>34</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -1425,74 +1416,74 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F57" s="10"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C58" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E58" s="8">
         <f>E55+1</f>
         <v>35</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C60" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="5"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D61" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E61" s="8">
         <f>E58+1</f>
         <v>36</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C62" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="5"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D63" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E63" s="8">
         <f>E61+1</f>
         <v>37</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -1504,268 +1495,268 @@
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C65" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D66" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E66" s="8">
         <f>E61</f>
         <v>36</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D67" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E67" s="8">
         <f>E61</f>
         <v>36</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D68" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E68" s="8">
         <f>E61</f>
         <v>36</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C69" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D70" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E70" s="8">
         <f>E63+1</f>
         <v>38</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D71" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E71" s="8">
         <f>E70</f>
         <v>38</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D72" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E72" s="8">
         <f>E70</f>
         <v>38</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D73" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E73" s="8">
         <f>E70</f>
         <v>38</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D74" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E74" s="8">
         <f>E70</f>
         <v>38</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C75" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="10"/>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D76" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E76" s="8">
         <f>E70+1</f>
         <v>39</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D77" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E77" s="8">
         <f>E76</f>
         <v>39</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D78" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E78" s="8">
         <f>E77</f>
         <v>39</v>
       </c>
       <c r="F78" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D79" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E79" s="8">
         <f>E78</f>
         <v>39</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D80" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E80" s="8">
         <f>E79</f>
         <v>39</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D81" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E81" s="8">
         <f>E80</f>
         <v>39</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C82" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D83" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E83" s="7">
         <f>E76+1</f>
         <v>40</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D84" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E84" s="7">
         <f>E83+1</f>
         <v>41</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.3">
@@ -1777,47 +1768,47 @@
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C86" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E86" s="8">
         <f>E84+1</f>
         <v>42</v>
       </c>
       <c r="F86" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C87" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E87" s="8">
         <f>E86+1</f>
         <v>43</v>
       </c>
       <c r="F87" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C88" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E88" s="8">
         <f>E87+1</f>
         <v>44</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.3">
@@ -1829,401 +1820,445 @@
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C90" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E90" s="8"/>
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D91" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E91" s="7">
         <f>E88+1</f>
         <v>45</v>
       </c>
       <c r="F91" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D92" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E92" s="7">
         <f>E91</f>
         <v>45</v>
       </c>
       <c r="F92" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D93" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E93" s="7">
         <f t="shared" ref="E93:E94" si="12">E92+1</f>
         <v>46</v>
       </c>
       <c r="F93" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D94" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E94" s="7">
         <f t="shared" si="12"/>
         <v>47</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C95" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F95" s="10"/>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D96" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E96" s="7">
         <f>E94+1</f>
         <v>48</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G96" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D97" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E97" s="7">
         <f>E96</f>
         <v>48</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G97" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="98" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D98" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E98" s="7">
         <f t="shared" ref="E98:E99" si="13">E97+1</f>
         <v>49</v>
       </c>
       <c r="F98" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="G98" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D99" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E99" s="7">
         <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="F99" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="G99" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="100" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C100" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="10"/>
     </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D101" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E101" s="7">
         <f>E99+1</f>
         <v>51</v>
       </c>
       <c r="F101" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G101" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="102" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D102" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E102" s="7">
         <f>E101</f>
         <v>51</v>
       </c>
       <c r="F102" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G102" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="103" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D103" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E103" s="7">
         <f t="shared" ref="E103:E104" si="14">E102+1</f>
         <v>52</v>
       </c>
       <c r="F103" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="G103" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="104" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D104" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E104" s="7">
         <f t="shared" si="14"/>
         <v>53</v>
       </c>
       <c r="F104" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="105" spans="3:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="G104" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="105" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C105" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F105" s="10"/>
     </row>
-    <row r="106" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D106" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E106" s="7">
         <f>E104+1</f>
         <v>54</v>
       </c>
       <c r="F106" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="107" spans="3:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G106" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="107" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D107" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E107" s="7">
         <f>E106</f>
         <v>54</v>
       </c>
       <c r="F107" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="108" spans="3:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G107" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="108" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D108" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E108" s="7">
         <f t="shared" ref="E108:E109" si="15">E107+1</f>
         <v>55</v>
       </c>
       <c r="F108" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="109" spans="3:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="G108" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="109" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D109" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E109" s="7">
         <f t="shared" si="15"/>
         <v>56</v>
       </c>
       <c r="F109" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="110" spans="3:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="G109" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="110" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C110" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D110" s="4"/>
       <c r="F110" s="10"/>
     </row>
-    <row r="111" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D111" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E111" s="7">
         <f>E109+1</f>
         <v>57</v>
       </c>
       <c r="F111" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="112" spans="3:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G111" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="112" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D112" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E112" s="7">
         <f>E111</f>
         <v>57</v>
       </c>
       <c r="F112" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G112" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D113" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E113" s="7">
         <f t="shared" ref="E113:E114" si="16">E112+1</f>
         <v>58</v>
       </c>
       <c r="F113" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="G113" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D114" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E114" s="7">
         <f t="shared" si="16"/>
         <v>59</v>
       </c>
       <c r="F114" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="G114" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C115" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E115" s="8"/>
       <c r="F115" s="10"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D116" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E116" s="7">
         <f>E114+1</f>
         <v>60</v>
       </c>
       <c r="F116" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D117" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E117" s="7">
         <f>E116</f>
         <v>60</v>
       </c>
       <c r="F117" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D118" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E118" s="7">
         <f t="shared" ref="E118:E119" si="17">E117+1</f>
         <v>61</v>
       </c>
       <c r="F118" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D119" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E119" s="7">
         <f t="shared" si="17"/>
         <v>62</v>
       </c>
       <c r="F119" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E120" s="8"/>
       <c r="F120" s="10"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C121" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E121" s="7">
+        <f>E119+1</f>
+        <v>63</v>
+      </c>
+      <c r="F121" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C122" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E122" s="7">
+        <f>E121+1</f>
+        <v>64</v>
+      </c>
+      <c r="F122" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C123" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E123" s="7">
+        <f t="shared" ref="E123:E124" si="18">E122+1</f>
+        <v>65</v>
+      </c>
+      <c r="F123" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C124" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F121" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C122" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F122" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C123" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F123" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C124" s="4" t="s">
-        <v>45</v>
+      <c r="E124" s="7">
+        <f t="shared" si="18"/>
+        <v>66</v>
       </c>
       <c r="F124" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15"/>
-      <c r="E125" s="16"/>
-      <c r="F125" s="17"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B126" t="s">
-        <v>20</v>
-      </c>
-      <c r="F126" s="10"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B127" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizado documento de pruebas
</commit_message>
<xml_diff>
--- a/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
+++ b/doc/capitulos/Anexos/Capítulo 8. Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xamel\Dropbox\Uniovi\TFG\ElFavorDeLasGuerreras\doc\capitulos\Anexos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF647A6-7147-4D42-B791-8667B93317D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA493DB-8D7D-41C9-A48E-2EB8B287D1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{91E62D61-3371-49A3-925F-74CADD294985}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="72">
   <si>
     <t>4 acciones libres</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Seleccionar accion seleccion</t>
   </si>
   <si>
-    <t>Finalizar turno</t>
-  </si>
-  <si>
     <t>No se ve la mano del adversario</t>
   </si>
   <si>
@@ -152,18 +149,6 @@
   </si>
   <si>
     <t>Todo vacío excepto las manos de los jugadores</t>
-  </si>
-  <si>
-    <t>No se han completado todas las acciones</t>
-  </si>
-  <si>
-    <t>Gana el jugador 1</t>
-  </si>
-  <si>
-    <t>Gana el jugador 2</t>
-  </si>
-  <si>
-    <t>Empate</t>
   </si>
   <si>
     <t>Tiene la mano con un solo hueco</t>
@@ -344,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -384,6 +369,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCFEB32-98DF-4F9A-96C0-42E72833AD6E}">
-  <dimension ref="A1:S124"/>
+  <dimension ref="A1:S119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="G104" sqref="G101:G104"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,16 +717,16 @@
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -768,54 +754,54 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="8">
         <v>1</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S5" s="18"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="8">
         <f>E5+1</f>
         <v>2</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S6" s="18"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="8">
         <f>E6+1</f>
         <v>3</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S7" s="18"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="10"/>
@@ -823,39 +809,39 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="8">
         <f>E7+1</f>
         <v>4</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S9" s="18"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="8">
         <f>E9+1</f>
         <v>5</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S10" s="18"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="10"/>
@@ -863,39 +849,39 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="8">
         <f t="shared" ref="E12" si="0">E10+1</f>
         <v>6</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S12" s="18"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="8">
         <f t="shared" ref="E13" si="1">E12+1</f>
         <v>7</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S13" s="18"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="10"/>
@@ -903,84 +889,84 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="8">
         <f t="shared" ref="E15" si="2">E13+1</f>
         <v>8</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="8">
         <f t="shared" ref="E16" si="3">E15+1</f>
         <v>9</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="8">
         <f t="shared" ref="E18" si="4">E16+1</f>
         <v>10</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" s="8">
         <f t="shared" ref="E19:E20" si="5">E18+1</f>
         <v>11</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="8">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1006,10 +992,10 @@
         <v>13</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1021,10 +1007,10 @@
         <v>14</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1036,10 +1022,10 @@
         <v>15</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1058,10 +1044,10 @@
         <v>16</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1073,10 +1059,10 @@
         <v>17</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -1103,210 +1089,210 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D32" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E32" s="8">
         <f>E28+1</f>
         <v>18</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D33" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E33" s="8">
         <f>E32+1</f>
         <v>19</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D34" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E34" s="8">
         <f>E33+1</f>
         <v>20</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C35" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="10"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D36" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E36" s="8">
         <f>E34+1</f>
         <v>21</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D37" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E37" s="8">
         <f>E36+1</f>
         <v>22</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="10"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D39" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E39" s="8">
         <f t="shared" ref="E39" si="6">E37+1</f>
         <v>23</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D40" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E40" s="8">
         <f t="shared" ref="E40" si="7">E39+1</f>
         <v>24</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="10"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D42" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E42" s="8">
         <f t="shared" ref="E42" si="8">E40+1</f>
         <v>25</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D43" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E43" s="8">
         <f t="shared" ref="E43" si="9">E42+1</f>
         <v>26</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="10"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D45" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E45" s="8">
         <f t="shared" ref="E45" si="10">E43+1</f>
         <v>27</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D46" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E46" s="8">
         <f t="shared" ref="E46:E47" si="11">E45+1</f>
         <v>28</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C47" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E47" s="8">
         <f t="shared" si="11"/>
         <v>29</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
@@ -1332,10 +1318,10 @@
         <v>30</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -1347,10 +1333,10 @@
         <v>31</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -1362,10 +1348,10 @@
         <v>32</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -1384,10 +1370,10 @@
         <v>33</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -1399,10 +1385,10 @@
         <v>34</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -1416,74 +1402,74 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F57" s="10"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C58" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E58" s="8">
         <f>E55+1</f>
         <v>35</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C60" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="5"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D61" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E61" s="8">
         <f>E58+1</f>
         <v>36</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C62" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="5"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D63" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E63" s="8">
         <f>E61+1</f>
         <v>37</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -1495,238 +1481,238 @@
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C65" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="5"/>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D66" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E66" s="8">
         <f>E61</f>
         <v>36</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D67" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E67" s="8">
         <f>E61</f>
         <v>36</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D68" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E68" s="8">
         <f>E61</f>
         <v>36</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C69" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D70" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E70" s="8">
         <f>E63+1</f>
         <v>38</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D71" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E71" s="8">
         <f>E70</f>
         <v>38</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D72" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E72" s="8">
         <f>E70</f>
         <v>38</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D73" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E73" s="8">
         <f>E70</f>
         <v>38</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D74" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E74" s="8">
         <f>E70</f>
         <v>38</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C75" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="10"/>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D76" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E76" s="8">
         <f>E70+1</f>
         <v>39</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D77" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E77" s="8">
         <f>E76</f>
         <v>39</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D78" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E78" s="8">
         <f>E77</f>
         <v>39</v>
       </c>
       <c r="F78" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D79" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E79" s="8">
         <f>E78</f>
         <v>39</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D80" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E80" s="8">
         <f>E79</f>
         <v>39</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D81" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E81" s="8">
         <f>E80</f>
         <v>39</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C82" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.3">
@@ -1738,10 +1724,10 @@
         <v>40</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.3">
@@ -1753,10 +1739,10 @@
         <v>41</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.3">
@@ -1768,47 +1754,47 @@
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C86" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E86" s="8">
         <f>E84+1</f>
         <v>42</v>
       </c>
       <c r="F86" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C87" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E87" s="8">
         <f>E86+1</f>
         <v>43</v>
       </c>
       <c r="F87" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C88" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E88" s="8">
         <f>E87+1</f>
         <v>44</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.3">
@@ -1820,445 +1806,404 @@
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C90" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E90" s="8"/>
       <c r="F90" s="5"/>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D91" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E91" s="7">
         <f>E88+1</f>
         <v>45</v>
       </c>
       <c r="F91" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D92" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E92" s="7">
         <f>E91</f>
         <v>45</v>
       </c>
       <c r="F92" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D93" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E93" s="7">
         <f t="shared" ref="E93:E94" si="12">E92+1</f>
         <v>46</v>
       </c>
       <c r="F93" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D94" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E94" s="7">
         <f t="shared" si="12"/>
         <v>47</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C95" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F95" s="10"/>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D96" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E96" s="7">
         <f>E94+1</f>
         <v>48</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G96" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D97" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E97" s="7">
         <f>E96</f>
         <v>48</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D98" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E98" s="7">
         <f t="shared" ref="E98:E99" si="13">E97+1</f>
         <v>49</v>
       </c>
       <c r="F98" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G98" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D99" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E99" s="7">
         <f t="shared" si="13"/>
         <v>50</v>
       </c>
       <c r="F99" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G99" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C100" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="10"/>
     </row>
     <row r="101" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D101" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E101" s="7">
         <f>E99+1</f>
         <v>51</v>
       </c>
       <c r="F101" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G101" s="11" t="s">
-        <v>69</v>
+        <v>34</v>
+      </c>
+      <c r="G101" s="19" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="102" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D102" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E102" s="7">
         <f>E101</f>
         <v>51</v>
       </c>
       <c r="F102" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G102" s="11" t="s">
-        <v>69</v>
+        <v>34</v>
+      </c>
+      <c r="G102" s="19" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="103" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D103" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E103" s="7">
         <f t="shared" ref="E103:E104" si="14">E102+1</f>
         <v>52</v>
       </c>
       <c r="F103" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G103" s="11" t="s">
-        <v>69</v>
+        <v>35</v>
+      </c>
+      <c r="G103" s="19" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="104" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D104" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E104" s="7">
         <f t="shared" si="14"/>
         <v>53</v>
       </c>
       <c r="F104" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G104" s="11" t="s">
-        <v>69</v>
+        <v>35</v>
+      </c>
+      <c r="G104" s="19" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="105" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C105" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F105" s="10"/>
     </row>
     <row r="106" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D106" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E106" s="7">
         <f>E104+1</f>
         <v>54</v>
       </c>
       <c r="F106" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G106" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D107" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E107" s="7">
         <f>E106</f>
         <v>54</v>
       </c>
       <c r="F107" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G107" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D108" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E108" s="7">
         <f t="shared" ref="E108:E109" si="15">E107+1</f>
         <v>55</v>
       </c>
       <c r="F108" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G108" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D109" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E109" s="7">
         <f t="shared" si="15"/>
         <v>56</v>
       </c>
       <c r="F109" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G109" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="110" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C110" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D110" s="4"/>
       <c r="F110" s="10"/>
+      <c r="G110" s="18"/>
     </row>
     <row r="111" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D111" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E111" s="7">
         <f>E109+1</f>
         <v>57</v>
       </c>
       <c r="F111" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G111" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="112" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D112" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E112" s="7">
         <f>E111</f>
         <v>57</v>
       </c>
       <c r="F112" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="113" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D113" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E113" s="7">
         <f t="shared" ref="E113:E114" si="16">E112+1</f>
         <v>58</v>
       </c>
       <c r="F113" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="114" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D114" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E114" s="7">
         <f t="shared" si="16"/>
         <v>59</v>
       </c>
       <c r="F114" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G114" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="115" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C115" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E115" s="8"/>
       <c r="F115" s="10"/>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G115" s="18"/>
+    </row>
+    <row r="116" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D116" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E116" s="7">
         <f>E114+1</f>
         <v>60</v>
       </c>
       <c r="F116" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="G116" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="117" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D117" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E117" s="7">
         <f>E116</f>
         <v>60</v>
       </c>
       <c r="F117" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="G117" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="118" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D118" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E118" s="7">
         <f t="shared" ref="E118:E119" si="17">E117+1</f>
         <v>61</v>
       </c>
       <c r="F118" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G118" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="119" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D119" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E119" s="7">
         <f t="shared" si="17"/>
         <v>62</v>
       </c>
       <c r="F119" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B120" t="s">
-        <v>19</v>
-      </c>
-      <c r="E120" s="8"/>
-      <c r="F120" s="10"/>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C121" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E121" s="7">
-        <f>E119+1</f>
-        <v>63</v>
-      </c>
-      <c r="F121" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C122" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E122" s="7">
-        <f>E121+1</f>
-        <v>64</v>
-      </c>
-      <c r="F122" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C123" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E123" s="7">
-        <f t="shared" ref="E123:E124" si="18">E122+1</f>
-        <v>65</v>
-      </c>
-      <c r="F123" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C124" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E124" s="7">
-        <f t="shared" si="18"/>
-        <v>66</v>
-      </c>
-      <c r="F124" s="10" t="s">
-        <v>35</v>
+      <c r="G119" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>